<commit_message>
correct errors in benchmark
</commit_message>
<xml_diff>
--- a/code_generate_figures/data/metrics_FragPipe_TMT_all_ensemble_mv.xlsx
+++ b/code_generate_figures/data/metrics_FragPipe_TMT_all_ensemble_mv.xlsx
@@ -69,15 +69,15 @@
     <t xml:space="preserve">pauc001_C.E_HYms2faims815_TMT16</t>
   </si>
   <si>
+    <t xml:space="preserve">pauc001_A.C_HYsps2815_TMT16</t>
+  </si>
+  <si>
     <t xml:space="preserve">pauc001_B.C_HYsps2815_TMT16</t>
   </si>
   <si>
     <t xml:space="preserve">pauc001_B.E_HYsps2815_TMT16</t>
   </si>
   <si>
-    <t xml:space="preserve">pauc001_A.C_HYsps2815_TMT16</t>
-  </si>
-  <si>
     <t xml:space="preserve">pauc001_A.D_HYms2815_TMT16</t>
   </si>
   <si>
@@ -246,15 +246,15 @@
     <t xml:space="preserve">pauc005_C.E_HYms2faims815_TMT16</t>
   </si>
   <si>
+    <t xml:space="preserve">pauc005_A.C_HYsps2815_TMT16</t>
+  </si>
+  <si>
     <t xml:space="preserve">pauc005_B.C_HYsps2815_TMT16</t>
   </si>
   <si>
     <t xml:space="preserve">pauc005_B.E_HYsps2815_TMT16</t>
   </si>
   <si>
-    <t xml:space="preserve">pauc005_A.C_HYsps2815_TMT16</t>
-  </si>
-  <si>
     <t xml:space="preserve">pauc005_A.D_HYms2815_TMT16</t>
   </si>
   <si>
@@ -291,15 +291,15 @@
     <t xml:space="preserve">pauc01_C.E_HYms2faims815_TMT16</t>
   </si>
   <si>
+    <t xml:space="preserve">pauc01_A.C_HYsps2815_TMT16</t>
+  </si>
+  <si>
     <t xml:space="preserve">pauc01_B.C_HYsps2815_TMT16</t>
   </si>
   <si>
     <t xml:space="preserve">pauc01_B.E_HYsps2815_TMT16</t>
   </si>
   <si>
-    <t xml:space="preserve">pauc01_A.C_HYsps2815_TMT16</t>
-  </si>
-  <si>
     <t xml:space="preserve">pauc01_A.D_HYms2815_TMT16</t>
   </si>
   <si>
@@ -336,15 +336,15 @@
     <t xml:space="preserve">nMcc_C.E_HYms2faims815_TMT16</t>
   </si>
   <si>
+    <t xml:space="preserve">nMcc_A.C_HYsps2815_TMT16</t>
+  </si>
+  <si>
     <t xml:space="preserve">nMcc_B.C_HYsps2815_TMT16</t>
   </si>
   <si>
     <t xml:space="preserve">nMcc_B.E_HYsps2815_TMT16</t>
   </si>
   <si>
-    <t xml:space="preserve">nMcc_A.C_HYsps2815_TMT16</t>
-  </si>
-  <si>
     <t xml:space="preserve">nMcc_A.D_HYms2815_TMT16</t>
   </si>
   <si>
@@ -381,15 +381,15 @@
     <t xml:space="preserve">geomean_C.E_HYms2faims815_TMT16</t>
   </si>
   <si>
+    <t xml:space="preserve">geomean_A.C_HYsps2815_TMT16</t>
+  </si>
+  <si>
     <t xml:space="preserve">geomean_B.C_HYsps2815_TMT16</t>
   </si>
   <si>
     <t xml:space="preserve">geomean_B.E_HYsps2815_TMT16</t>
   </si>
   <si>
-    <t xml:space="preserve">geomean_A.C_HYsps2815_TMT16</t>
-  </si>
-  <si>
     <t xml:space="preserve">geomean_A.D_HYms2815_TMT16</t>
   </si>
   <si>
@@ -432,13 +432,13 @@
     <t xml:space="preserve">conditionC-conditionE</t>
   </si>
   <si>
+    <t xml:space="preserve">conditionA-conditionC</t>
+  </si>
+  <si>
     <t xml:space="preserve">conditionB-conditionC</t>
   </si>
   <si>
     <t xml:space="preserve">conditionB-conditionE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">conditionA-conditionC</t>
   </si>
   <si>
     <t xml:space="preserve">conditionA-conditionD</t>
@@ -930,13 +930,13 @@
         <v>0.8096417</v>
       </c>
       <c r="X2" t="n">
-        <v>0.79441905</v>
+        <v>0.7888409</v>
       </c>
       <c r="Y2" t="n">
         <v>7</v>
       </c>
       <c r="Z2" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3">
@@ -1010,7 +1010,7 @@
         <v>0.80244478</v>
       </c>
       <c r="X3" t="n">
-        <v>0.7953596</v>
+        <v>0.7936414</v>
       </c>
       <c r="Y3" t="n">
         <v>18</v>
@@ -1090,7 +1090,7 @@
         <v>0.808257533333333</v>
       </c>
       <c r="X4" t="n">
-        <v>0.79691425</v>
+        <v>0.7961511</v>
       </c>
       <c r="Y4" t="n">
         <v>16</v>
@@ -1170,13 +1170,13 @@
         <v>0.8090653</v>
       </c>
       <c r="X5" t="n">
-        <v>0.79428695</v>
+        <v>0.7885364</v>
       </c>
       <c r="Y5" t="n">
         <v>12</v>
       </c>
       <c r="Z5" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6">
@@ -1250,13 +1250,13 @@
         <v>0.80883304</v>
       </c>
       <c r="X6" t="n">
-        <v>0.79400635</v>
+        <v>0.7885344</v>
       </c>
       <c r="Y6" t="n">
         <v>15</v>
       </c>
       <c r="Z6" t="n">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7">
@@ -1330,13 +1330,13 @@
         <v>0.808886206666667</v>
       </c>
       <c r="X7" t="n">
-        <v>0.7940528</v>
+        <v>0.7885344</v>
       </c>
       <c r="Y7" t="n">
         <v>14</v>
       </c>
       <c r="Z7" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8">
@@ -1410,13 +1410,13 @@
         <v>0.809472093333333</v>
       </c>
       <c r="X8" t="n">
-        <v>0.7941767</v>
+        <v>0.7888388</v>
       </c>
       <c r="Y8" t="n">
         <v>8</v>
       </c>
       <c r="Z8" t="n">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9">
@@ -1490,7 +1490,7 @@
         <v>0.802411993333333</v>
       </c>
       <c r="X9" t="n">
-        <v>0.7953475</v>
+        <v>0.7936414</v>
       </c>
       <c r="Y9" t="n">
         <v>20</v>
@@ -1570,7 +1570,7 @@
         <v>0.808217526666667</v>
       </c>
       <c r="X10" t="n">
-        <v>0.7967578</v>
+        <v>0.7959714</v>
       </c>
       <c r="Y10" t="n">
         <v>17</v>
@@ -1650,13 +1650,13 @@
         <v>0.8096693</v>
       </c>
       <c r="X11" t="n">
-        <v>0.7944392</v>
+        <v>0.7888409</v>
       </c>
       <c r="Y11" t="n">
         <v>6</v>
       </c>
       <c r="Z11" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12">
@@ -1730,7 +1730,7 @@
         <v>0.802414973333333</v>
       </c>
       <c r="X12" t="n">
-        <v>0.7953475</v>
+        <v>0.7936414</v>
       </c>
       <c r="Y12" t="n">
         <v>19</v>
@@ -1810,13 +1810,13 @@
         <v>0.808942486666667</v>
       </c>
       <c r="X13" t="n">
-        <v>0.79400635</v>
+        <v>0.7885344</v>
       </c>
       <c r="Y13" t="n">
         <v>13</v>
       </c>
       <c r="Z13" t="n">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14">
@@ -1890,7 +1890,7 @@
         <v>0.820712733333333</v>
       </c>
       <c r="X14" t="n">
-        <v>0.80511515</v>
+        <v>0.8015114</v>
       </c>
       <c r="Y14" t="n">
         <v>2</v>
@@ -1970,13 +1970,13 @@
         <v>0.80939674</v>
       </c>
       <c r="X15" t="n">
-        <v>0.79417805</v>
+        <v>0.7884538</v>
       </c>
       <c r="Y15" t="n">
         <v>11</v>
       </c>
       <c r="Z15" t="n">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16">
@@ -2050,7 +2050,7 @@
         <v>0.820587686666667</v>
       </c>
       <c r="X16" t="n">
-        <v>0.80443175</v>
+        <v>0.8005746</v>
       </c>
       <c r="Y16" t="n">
         <v>4</v>
@@ -2130,7 +2130,7 @@
         <v>0.813047833333333</v>
       </c>
       <c r="X17" t="n">
-        <v>0.80110285</v>
+        <v>0.7964122</v>
       </c>
       <c r="Y17" t="n">
         <v>5</v>
@@ -2210,7 +2210,7 @@
         <v>0.82073002</v>
       </c>
       <c r="X18" t="n">
-        <v>0.80512925</v>
+        <v>0.8016446</v>
       </c>
       <c r="Y18" t="n">
         <v>1</v>
@@ -2290,13 +2290,13 @@
         <v>0.809399373333333</v>
       </c>
       <c r="X19" t="n">
-        <v>0.7941791</v>
+        <v>0.7884559</v>
       </c>
       <c r="Y19" t="n">
         <v>10</v>
       </c>
       <c r="Z19" t="n">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="20">
@@ -2370,7 +2370,7 @@
         <v>0.820601613333333</v>
       </c>
       <c r="X20" t="n">
-        <v>0.80444185</v>
+        <v>0.800724</v>
       </c>
       <c r="Y20" t="n">
         <v>3</v>
@@ -2450,7 +2450,7 @@
         <v>0.809407486666667</v>
       </c>
       <c r="X21" t="n">
-        <v>0.80111445</v>
+        <v>0.7964637</v>
       </c>
       <c r="Y21" t="n">
         <v>9</v>
@@ -2624,13 +2624,13 @@
         <v>0.909427526666667</v>
       </c>
       <c r="X2" t="n">
-        <v>0.91704015</v>
+        <v>0.9178586</v>
       </c>
       <c r="Y2" t="n">
         <v>9</v>
       </c>
       <c r="Z2" t="n">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3">
@@ -2704,7 +2704,7 @@
         <v>0.903682886666667</v>
       </c>
       <c r="X3" t="n">
-        <v>0.92075195</v>
+        <v>0.9209819</v>
       </c>
       <c r="Y3" t="n">
         <v>18</v>
@@ -2784,13 +2784,13 @@
         <v>0.907436913333333</v>
       </c>
       <c r="X4" t="n">
-        <v>0.92190315</v>
+        <v>0.9225368</v>
       </c>
       <c r="Y4" t="n">
         <v>13</v>
       </c>
       <c r="Z4" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5">
@@ -2864,13 +2864,13 @@
         <v>0.907338753333333</v>
       </c>
       <c r="X5" t="n">
-        <v>0.91488075</v>
+        <v>0.9159912</v>
       </c>
       <c r="Y5" t="n">
         <v>15</v>
       </c>
       <c r="Z5" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6">
@@ -2944,13 +2944,13 @@
         <v>0.907288666666667</v>
       </c>
       <c r="X6" t="n">
-        <v>0.91481085</v>
+        <v>0.915987</v>
       </c>
       <c r="Y6" t="n">
         <v>17</v>
       </c>
       <c r="Z6" t="n">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7">
@@ -3024,13 +3024,13 @@
         <v>0.90731232</v>
       </c>
       <c r="X7" t="n">
-        <v>0.91484495</v>
+        <v>0.915987</v>
       </c>
       <c r="Y7" t="n">
         <v>16</v>
       </c>
       <c r="Z7" t="n">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8">
@@ -3104,13 +3104,13 @@
         <v>0.909446706666667</v>
       </c>
       <c r="X8" t="n">
-        <v>0.9170626</v>
+        <v>0.9178557</v>
       </c>
       <c r="Y8" t="n">
         <v>7</v>
       </c>
       <c r="Z8" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9">
@@ -3184,7 +3184,7 @@
         <v>0.903669606666667</v>
       </c>
       <c r="X9" t="n">
-        <v>0.9207336</v>
+        <v>0.9209819</v>
       </c>
       <c r="Y9" t="n">
         <v>19</v>
@@ -3264,7 +3264,7 @@
         <v>0.907433593333333</v>
       </c>
       <c r="X10" t="n">
-        <v>0.92191035</v>
+        <v>0.9225368</v>
       </c>
       <c r="Y10" t="n">
         <v>14</v>
@@ -3344,13 +3344,13 @@
         <v>0.909439033333333</v>
       </c>
       <c r="X11" t="n">
-        <v>0.91711615</v>
+        <v>0.9178574</v>
       </c>
       <c r="Y11" t="n">
         <v>8</v>
       </c>
       <c r="Z11" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12">
@@ -3424,7 +3424,7 @@
         <v>0.903658266666667</v>
       </c>
       <c r="X12" t="n">
-        <v>0.9207336</v>
+        <v>0.9209819</v>
       </c>
       <c r="Y12" t="n">
         <v>20</v>
@@ -3504,13 +3504,13 @@
         <v>0.90750886</v>
       </c>
       <c r="X13" t="n">
-        <v>0.91526995</v>
+        <v>0.9159293</v>
       </c>
       <c r="Y13" t="n">
         <v>10</v>
       </c>
       <c r="Z13" t="n">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14">
@@ -3584,13 +3584,13 @@
         <v>0.916823973333333</v>
       </c>
       <c r="X14" t="n">
-        <v>0.9246317</v>
+        <v>0.9246578</v>
       </c>
       <c r="Y14" t="n">
         <v>1</v>
       </c>
       <c r="Z14" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15">
@@ -3664,13 +3664,13 @@
         <v>0.907439473333333</v>
       </c>
       <c r="X15" t="n">
-        <v>0.91485475</v>
+        <v>0.9159723</v>
       </c>
       <c r="Y15" t="n">
         <v>12</v>
       </c>
       <c r="Z15" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16">
@@ -3744,7 +3744,7 @@
         <v>0.91682126</v>
       </c>
       <c r="X16" t="n">
-        <v>0.9246463</v>
+        <v>0.9246582</v>
       </c>
       <c r="Y16" t="n">
         <v>2</v>
@@ -3824,7 +3824,7 @@
         <v>0.914007273333333</v>
       </c>
       <c r="X17" t="n">
-        <v>0.9229781</v>
+        <v>0.923434</v>
       </c>
       <c r="Y17" t="n">
         <v>5</v>
@@ -3904,7 +3904,7 @@
         <v>0.9168181</v>
       </c>
       <c r="X18" t="n">
-        <v>0.92462335</v>
+        <v>0.9246262</v>
       </c>
       <c r="Y18" t="n">
         <v>3</v>
@@ -3984,13 +3984,13 @@
         <v>0.90744096</v>
       </c>
       <c r="X19" t="n">
-        <v>0.9148555</v>
+        <v>0.9159727</v>
       </c>
       <c r="Y19" t="n">
         <v>11</v>
       </c>
       <c r="Z19" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="20">
@@ -4064,13 +4064,13 @@
         <v>0.916813173333333</v>
       </c>
       <c r="X20" t="n">
-        <v>0.9246371</v>
+        <v>0.9246567</v>
       </c>
       <c r="Y20" t="n">
         <v>4</v>
       </c>
       <c r="Z20" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21">
@@ -4144,13 +4144,13 @@
         <v>0.912969446666667</v>
       </c>
       <c r="X21" t="n">
-        <v>0.9221578</v>
+        <v>0.922374</v>
       </c>
       <c r="Y21" t="n">
         <v>6</v>
       </c>
       <c r="Z21" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -4318,7 +4318,7 @@
         <v>0.931565153333333</v>
       </c>
       <c r="X2" t="n">
-        <v>0.94214915</v>
+        <v>0.9430005</v>
       </c>
       <c r="Y2" t="n">
         <v>9</v>
@@ -4398,7 +4398,7 @@
         <v>0.927350286666667</v>
       </c>
       <c r="X3" t="n">
-        <v>0.93985615</v>
+        <v>0.9427314</v>
       </c>
       <c r="Y3" t="n">
         <v>18</v>
@@ -4478,7 +4478,7 @@
         <v>0.9305309</v>
       </c>
       <c r="X4" t="n">
-        <v>0.9422897</v>
+        <v>0.9444176</v>
       </c>
       <c r="Y4" t="n">
         <v>10</v>
@@ -4558,13 +4558,13 @@
         <v>0.92906686</v>
       </c>
       <c r="X5" t="n">
-        <v>0.9412983</v>
+        <v>0.9428095</v>
       </c>
       <c r="Y5" t="n">
         <v>15</v>
       </c>
       <c r="Z5" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6">
@@ -4638,7 +4638,7 @@
         <v>0.928965333333333</v>
       </c>
       <c r="X6" t="n">
-        <v>0.9412973</v>
+        <v>0.9428095</v>
       </c>
       <c r="Y6" t="n">
         <v>17</v>
@@ -4718,7 +4718,7 @@
         <v>0.928991786666667</v>
       </c>
       <c r="X7" t="n">
-        <v>0.9412972</v>
+        <v>0.9428095</v>
       </c>
       <c r="Y7" t="n">
         <v>16</v>
@@ -4798,13 +4798,13 @@
         <v>0.931565426666667</v>
       </c>
       <c r="X8" t="n">
-        <v>0.9421483</v>
+        <v>0.9430005</v>
       </c>
       <c r="Y8" t="n">
         <v>8</v>
       </c>
       <c r="Z8" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9">
@@ -4878,13 +4878,13 @@
         <v>0.92731006</v>
       </c>
       <c r="X9" t="n">
-        <v>0.9399158</v>
+        <v>0.9427301</v>
       </c>
       <c r="Y9" t="n">
         <v>19</v>
       </c>
       <c r="Z9" t="n">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10">
@@ -4958,7 +4958,7 @@
         <v>0.930503346666667</v>
       </c>
       <c r="X10" t="n">
-        <v>0.94236565</v>
+        <v>0.9444582</v>
       </c>
       <c r="Y10" t="n">
         <v>11</v>
@@ -5038,13 +5038,13 @@
         <v>0.931570833333333</v>
       </c>
       <c r="X11" t="n">
-        <v>0.9421487</v>
+        <v>0.9430005</v>
       </c>
       <c r="Y11" t="n">
         <v>7</v>
       </c>
       <c r="Z11" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12">
@@ -5118,13 +5118,13 @@
         <v>0.9272993</v>
       </c>
       <c r="X12" t="n">
-        <v>0.9398235</v>
+        <v>0.9427623</v>
       </c>
       <c r="Y12" t="n">
         <v>20</v>
       </c>
       <c r="Z12" t="n">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13">
@@ -5198,13 +5198,13 @@
         <v>0.929332033333333</v>
       </c>
       <c r="X13" t="n">
-        <v>0.9412543</v>
+        <v>0.942742</v>
       </c>
       <c r="Y13" t="n">
         <v>12</v>
       </c>
       <c r="Z13" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14">
@@ -5278,7 +5278,7 @@
         <v>0.938327093333333</v>
       </c>
       <c r="X14" t="n">
-        <v>0.94646955</v>
+        <v>0.9470992</v>
       </c>
       <c r="Y14" t="n">
         <v>1</v>
@@ -5358,13 +5358,13 @@
         <v>0.929085733333333</v>
       </c>
       <c r="X15" t="n">
-        <v>0.9412982</v>
+        <v>0.9428186</v>
       </c>
       <c r="Y15" t="n">
         <v>14</v>
       </c>
       <c r="Z15" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16">
@@ -5438,7 +5438,7 @@
         <v>0.93831254</v>
       </c>
       <c r="X16" t="n">
-        <v>0.94650545</v>
+        <v>0.9471593</v>
       </c>
       <c r="Y16" t="n">
         <v>2</v>
@@ -5518,7 +5518,7 @@
         <v>0.93590476</v>
       </c>
       <c r="X17" t="n">
-        <v>0.9454436</v>
+        <v>0.9465523</v>
       </c>
       <c r="Y17" t="n">
         <v>5</v>
@@ -5598,7 +5598,7 @@
         <v>0.938219746666667</v>
       </c>
       <c r="X18" t="n">
-        <v>0.9462816</v>
+        <v>0.9468049</v>
       </c>
       <c r="Y18" t="n">
         <v>3</v>
@@ -5678,7 +5678,7 @@
         <v>0.92908642</v>
       </c>
       <c r="X19" t="n">
-        <v>0.94130695</v>
+        <v>0.9428359</v>
       </c>
       <c r="Y19" t="n">
         <v>13</v>
@@ -5758,7 +5758,7 @@
         <v>0.938205893333333</v>
       </c>
       <c r="X20" t="n">
-        <v>0.94630455</v>
+        <v>0.9468523</v>
       </c>
       <c r="Y20" t="n">
         <v>4</v>
@@ -5838,7 +5838,7 @@
         <v>0.935214846666667</v>
       </c>
       <c r="X21" t="n">
-        <v>0.9449506</v>
+        <v>0.945688</v>
       </c>
       <c r="Y21" t="n">
         <v>6</v>
@@ -6012,13 +6012,13 @@
         <v>0.89093226</v>
       </c>
       <c r="X2" t="n">
-        <v>0.93851345</v>
+        <v>0.9414634</v>
       </c>
       <c r="Y2" t="n">
         <v>8</v>
       </c>
       <c r="Z2" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3">
@@ -6092,7 +6092,7 @@
         <v>0.83225362</v>
       </c>
       <c r="X3" t="n">
-        <v>0.92417105</v>
+        <v>0.9250249</v>
       </c>
       <c r="Y3" t="n">
         <v>18</v>
@@ -6172,7 +6172,7 @@
         <v>0.856910493333333</v>
       </c>
       <c r="X4" t="n">
-        <v>0.93556295</v>
+        <v>0.9362137</v>
       </c>
       <c r="Y4" t="n">
         <v>16</v>
@@ -6252,7 +6252,7 @@
         <v>0.873997206666667</v>
       </c>
       <c r="X5" t="n">
-        <v>0.93178775</v>
+        <v>0.9320369</v>
       </c>
       <c r="Y5" t="n">
         <v>13</v>
@@ -6332,7 +6332,7 @@
         <v>0.8739779</v>
       </c>
       <c r="X6" t="n">
-        <v>0.93178775</v>
+        <v>0.9320369</v>
       </c>
       <c r="Y6" t="n">
         <v>14</v>
@@ -6412,7 +6412,7 @@
         <v>0.873969193333333</v>
       </c>
       <c r="X7" t="n">
-        <v>0.93178775</v>
+        <v>0.9320369</v>
       </c>
       <c r="Y7" t="n">
         <v>15</v>
@@ -6492,13 +6492,13 @@
         <v>0.89091974</v>
       </c>
       <c r="X8" t="n">
-        <v>0.93851345</v>
+        <v>0.9414634</v>
       </c>
       <c r="Y8" t="n">
         <v>10</v>
       </c>
       <c r="Z8" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9">
@@ -6572,7 +6572,7 @@
         <v>0.832217713333333</v>
       </c>
       <c r="X9" t="n">
-        <v>0.92417105</v>
+        <v>0.9250249</v>
       </c>
       <c r="Y9" t="n">
         <v>19</v>
@@ -6652,7 +6652,7 @@
         <v>0.856842646666667</v>
       </c>
       <c r="X10" t="n">
-        <v>0.93546645</v>
+        <v>0.9362137</v>
       </c>
       <c r="Y10" t="n">
         <v>17</v>
@@ -6732,13 +6732,13 @@
         <v>0.89093226</v>
       </c>
       <c r="X11" t="n">
-        <v>0.93851345</v>
+        <v>0.9414634</v>
       </c>
       <c r="Y11" t="n">
         <v>9</v>
       </c>
       <c r="Z11" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12">
@@ -6812,7 +6812,7 @@
         <v>0.832217713333333</v>
       </c>
       <c r="X12" t="n">
-        <v>0.92417105</v>
+        <v>0.9250249</v>
       </c>
       <c r="Y12" t="n">
         <v>20</v>
@@ -6892,7 +6892,7 @@
         <v>0.895658306666667</v>
       </c>
       <c r="X13" t="n">
-        <v>0.94212565</v>
+        <v>0.942429</v>
       </c>
       <c r="Y13" t="n">
         <v>1</v>
@@ -6972,13 +6972,13 @@
         <v>0.89381102</v>
       </c>
       <c r="X14" t="n">
-        <v>0.93907895</v>
+        <v>0.9410196</v>
       </c>
       <c r="Y14" t="n">
         <v>5</v>
       </c>
       <c r="Z14" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15">
@@ -7052,7 +7052,7 @@
         <v>0.875396013333333</v>
       </c>
       <c r="X15" t="n">
-        <v>0.93178775</v>
+        <v>0.9320369</v>
       </c>
       <c r="Y15" t="n">
         <v>11</v>
@@ -7132,13 +7132,13 @@
         <v>0.89381378</v>
       </c>
       <c r="X16" t="n">
-        <v>0.93907895</v>
+        <v>0.9410196</v>
       </c>
       <c r="Y16" t="n">
         <v>4</v>
       </c>
       <c r="Z16" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17">
@@ -7212,7 +7212,7 @@
         <v>0.894040246666667</v>
       </c>
       <c r="X17" t="n">
-        <v>0.937956</v>
+        <v>0.9395342</v>
       </c>
       <c r="Y17" t="n">
         <v>3</v>
@@ -7292,13 +7292,13 @@
         <v>0.893710266666667</v>
       </c>
       <c r="X18" t="n">
-        <v>0.9390647</v>
+        <v>0.9414264</v>
       </c>
       <c r="Y18" t="n">
         <v>7</v>
       </c>
       <c r="Z18" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19">
@@ -7372,7 +7372,7 @@
         <v>0.875342833333333</v>
       </c>
       <c r="X19" t="n">
-        <v>0.93178775</v>
+        <v>0.9320369</v>
       </c>
       <c r="Y19" t="n">
         <v>12</v>
@@ -7452,13 +7452,13 @@
         <v>0.893738113333333</v>
       </c>
       <c r="X20" t="n">
-        <v>0.9390647</v>
+        <v>0.9414264</v>
       </c>
       <c r="Y20" t="n">
         <v>6</v>
       </c>
       <c r="Z20" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="21">
@@ -7532,13 +7532,13 @@
         <v>0.89406628</v>
       </c>
       <c r="X21" t="n">
-        <v>0.93865375</v>
+        <v>0.9407398</v>
       </c>
       <c r="Y21" t="n">
         <v>2</v>
       </c>
       <c r="Z21" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -7706,13 +7706,13 @@
         <v>0.84121464</v>
       </c>
       <c r="X2" t="n">
-        <v>0.92478745</v>
+        <v>0.9276481</v>
       </c>
       <c r="Y2" t="n">
         <v>8</v>
       </c>
       <c r="Z2" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3">
@@ -7786,7 +7786,7 @@
         <v>0.70849624</v>
       </c>
       <c r="X3" t="n">
-        <v>0.91289815</v>
+        <v>0.9146945</v>
       </c>
       <c r="Y3" t="n">
         <v>18</v>
@@ -7866,7 +7866,7 @@
         <v>0.7614179</v>
       </c>
       <c r="X4" t="n">
-        <v>0.9158146</v>
+        <v>0.9178386</v>
       </c>
       <c r="Y4" t="n">
         <v>16</v>
@@ -7946,13 +7946,13 @@
         <v>0.7866099</v>
       </c>
       <c r="X5" t="n">
-        <v>0.9220246</v>
+        <v>0.9275773</v>
       </c>
       <c r="Y5" t="n">
         <v>13</v>
       </c>
       <c r="Z5" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6">
@@ -8026,13 +8026,13 @@
         <v>0.78654014</v>
       </c>
       <c r="X6" t="n">
-        <v>0.9218614</v>
+        <v>0.9272509</v>
       </c>
       <c r="Y6" t="n">
         <v>14</v>
       </c>
       <c r="Z6" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7">
@@ -8106,13 +8106,13 @@
         <v>0.786536593333333</v>
       </c>
       <c r="X7" t="n">
-        <v>0.9218614</v>
+        <v>0.9272509</v>
       </c>
       <c r="Y7" t="n">
         <v>15</v>
       </c>
       <c r="Z7" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8">
@@ -8186,13 +8186,13 @@
         <v>0.841193453333333</v>
       </c>
       <c r="X8" t="n">
-        <v>0.92478745</v>
+        <v>0.9276481</v>
       </c>
       <c r="Y8" t="n">
         <v>10</v>
       </c>
       <c r="Z8" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9">
@@ -8266,7 +8266,7 @@
         <v>0.708422533333333</v>
       </c>
       <c r="X9" t="n">
-        <v>0.91272055</v>
+        <v>0.9146945</v>
       </c>
       <c r="Y9" t="n">
         <v>19</v>
@@ -8346,7 +8346,7 @@
         <v>0.761297613333333</v>
       </c>
       <c r="X10" t="n">
-        <v>0.915755</v>
+        <v>0.9177194</v>
       </c>
       <c r="Y10" t="n">
         <v>17</v>
@@ -8426,13 +8426,13 @@
         <v>0.84121464</v>
       </c>
       <c r="X11" t="n">
-        <v>0.92478745</v>
+        <v>0.9276481</v>
       </c>
       <c r="Y11" t="n">
         <v>9</v>
       </c>
       <c r="Z11" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12">
@@ -8506,7 +8506,7 @@
         <v>0.708422533333333</v>
       </c>
       <c r="X12" t="n">
-        <v>0.91272055</v>
+        <v>0.9146945</v>
       </c>
       <c r="Y12" t="n">
         <v>20</v>
@@ -8586,13 +8586,13 @@
         <v>0.843080133333333</v>
       </c>
       <c r="X13" t="n">
-        <v>0.92250415</v>
+        <v>0.9232219</v>
       </c>
       <c r="Y13" t="n">
         <v>7</v>
       </c>
       <c r="Z13" t="n">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14">
@@ -8666,7 +8666,7 @@
         <v>0.8474131</v>
       </c>
       <c r="X14" t="n">
-        <v>0.9273298</v>
+        <v>0.9327328</v>
       </c>
       <c r="Y14" t="n">
         <v>3</v>
@@ -8746,13 +8746,13 @@
         <v>0.79019768</v>
       </c>
       <c r="X15" t="n">
-        <v>0.92402075</v>
+        <v>0.9293631</v>
       </c>
       <c r="Y15" t="n">
         <v>11</v>
       </c>
       <c r="Z15" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16">
@@ -8826,7 +8826,7 @@
         <v>0.847399286666667</v>
       </c>
       <c r="X16" t="n">
-        <v>0.9273879</v>
+        <v>0.932849</v>
       </c>
       <c r="Y16" t="n">
         <v>4</v>
@@ -8906,7 +8906,7 @@
         <v>0.84829616</v>
       </c>
       <c r="X17" t="n">
-        <v>0.9277899</v>
+        <v>0.933653</v>
       </c>
       <c r="Y17" t="n">
         <v>1</v>
@@ -8986,7 +8986,7 @@
         <v>0.84717898</v>
       </c>
       <c r="X18" t="n">
-        <v>0.9275026</v>
+        <v>0.9330784</v>
       </c>
       <c r="Y18" t="n">
         <v>6</v>
@@ -9066,13 +9066,13 @@
         <v>0.790043546666667</v>
       </c>
       <c r="X19" t="n">
-        <v>0.9239375</v>
+        <v>0.9293631</v>
       </c>
       <c r="Y19" t="n">
         <v>12</v>
       </c>
       <c r="Z19" t="n">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20">
@@ -9146,7 +9146,7 @@
         <v>0.847195033333333</v>
       </c>
       <c r="X20" t="n">
-        <v>0.92756075</v>
+        <v>0.9331947</v>
       </c>
       <c r="Y20" t="n">
         <v>5</v>
@@ -9226,7 +9226,7 @@
         <v>0.848203893333333</v>
       </c>
       <c r="X21" t="n">
-        <v>0.9276172</v>
+        <v>0.9333076</v>
       </c>
       <c r="Y21" t="n">
         <v>2</v>
@@ -9400,7 +9400,7 @@
         <v>0.89258882</v>
       </c>
       <c r="X2" t="n">
-        <v>0.93613695</v>
+        <v>0.9374105</v>
       </c>
       <c r="Y2" t="n">
         <v>6</v>
@@ -9480,13 +9480,13 @@
         <v>0.884352813333333</v>
       </c>
       <c r="X3" t="n">
-        <v>0.93963285</v>
+        <v>0.939803</v>
       </c>
       <c r="Y3" t="n">
         <v>13</v>
       </c>
       <c r="Z3" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4">
@@ -9560,13 +9560,13 @@
         <v>0.885323453333333</v>
       </c>
       <c r="X4" t="n">
-        <v>0.93864615</v>
+        <v>0.9401447</v>
       </c>
       <c r="Y4" t="n">
         <v>11</v>
       </c>
       <c r="Z4" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5">
@@ -9640,7 +9640,7 @@
         <v>0.87526566</v>
       </c>
       <c r="X5" t="n">
-        <v>0.93178775</v>
+        <v>0.9320369</v>
       </c>
       <c r="Y5" t="n">
         <v>20</v>
@@ -9720,7 +9720,7 @@
         <v>0.875267026666667</v>
       </c>
       <c r="X6" t="n">
-        <v>0.93178775</v>
+        <v>0.9320369</v>
       </c>
       <c r="Y6" t="n">
         <v>19</v>
@@ -9800,7 +9800,7 @@
         <v>0.87528302</v>
       </c>
       <c r="X7" t="n">
-        <v>0.93178775</v>
+        <v>0.9320369</v>
       </c>
       <c r="Y7" t="n">
         <v>17</v>
@@ -9880,7 +9880,7 @@
         <v>0.89258882</v>
       </c>
       <c r="X8" t="n">
-        <v>0.93613695</v>
+        <v>0.9374105</v>
       </c>
       <c r="Y8" t="n">
         <v>7</v>
@@ -9960,13 +9960,13 @@
         <v>0.884334</v>
       </c>
       <c r="X9" t="n">
-        <v>0.93958475</v>
+        <v>0.9396098</v>
       </c>
       <c r="Y9" t="n">
         <v>14</v>
       </c>
       <c r="Z9" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10">
@@ -10040,13 +10040,13 @@
         <v>0.885293673333333</v>
       </c>
       <c r="X10" t="n">
-        <v>0.938594</v>
+        <v>0.9397074</v>
       </c>
       <c r="Y10" t="n">
         <v>12</v>
       </c>
       <c r="Z10" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11">
@@ -10120,7 +10120,7 @@
         <v>0.89258882</v>
       </c>
       <c r="X11" t="n">
-        <v>0.93613695</v>
+        <v>0.9374105</v>
       </c>
       <c r="Y11" t="n">
         <v>8</v>
@@ -10200,13 +10200,13 @@
         <v>0.884334</v>
       </c>
       <c r="X12" t="n">
-        <v>0.93958475</v>
+        <v>0.9396098</v>
       </c>
       <c r="Y12" t="n">
         <v>15</v>
       </c>
       <c r="Z12" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13">
@@ -10280,7 +10280,7 @@
         <v>0.896366746666667</v>
       </c>
       <c r="X13" t="n">
-        <v>0.94069075</v>
+        <v>0.9414732</v>
       </c>
       <c r="Y13" t="n">
         <v>1</v>
@@ -10360,7 +10360,7 @@
         <v>0.892636026666667</v>
       </c>
       <c r="X14" t="n">
-        <v>0.9363377</v>
+        <v>0.937812</v>
       </c>
       <c r="Y14" t="n">
         <v>4</v>
@@ -10440,7 +10440,7 @@
         <v>0.87527432</v>
       </c>
       <c r="X15" t="n">
-        <v>0.93178775</v>
+        <v>0.9320369</v>
       </c>
       <c r="Y15" t="n">
         <v>18</v>
@@ -10520,7 +10520,7 @@
         <v>0.892627066666667</v>
       </c>
       <c r="X16" t="n">
-        <v>0.9363377</v>
+        <v>0.937812</v>
       </c>
       <c r="Y16" t="n">
         <v>5</v>
@@ -10600,7 +10600,7 @@
         <v>0.8925635</v>
       </c>
       <c r="X17" t="n">
-        <v>0.9365667</v>
+        <v>0.9380812</v>
       </c>
       <c r="Y17" t="n">
         <v>9</v>
@@ -10680,7 +10680,7 @@
         <v>0.892657093333333</v>
       </c>
       <c r="X18" t="n">
-        <v>0.93627035</v>
+        <v>0.9376773</v>
       </c>
       <c r="Y18" t="n">
         <v>2</v>
@@ -10760,7 +10760,7 @@
         <v>0.87537476</v>
       </c>
       <c r="X19" t="n">
-        <v>0.93178775</v>
+        <v>0.9320369</v>
       </c>
       <c r="Y19" t="n">
         <v>16</v>
@@ -10840,7 +10840,7 @@
         <v>0.892648146666667</v>
       </c>
       <c r="X20" t="n">
-        <v>0.93627035</v>
+        <v>0.9376773</v>
       </c>
       <c r="Y20" t="n">
         <v>3</v>
@@ -10920,7 +10920,7 @@
         <v>0.89254254</v>
       </c>
       <c r="X21" t="n">
-        <v>0.9364994</v>
+        <v>0.9379466</v>
       </c>
       <c r="Y21" t="n">
         <v>10</v>
@@ -11094,7 +11094,7 @@
         <v>0.847183286666667</v>
       </c>
       <c r="X2" t="n">
-        <v>0.9280186</v>
+        <v>0.9341104</v>
       </c>
       <c r="Y2" t="n">
         <v>8</v>
@@ -11174,13 +11174,13 @@
         <v>0.82081226</v>
       </c>
       <c r="X3" t="n">
-        <v>0.91829245</v>
+        <v>0.9194454</v>
       </c>
       <c r="Y3" t="n">
         <v>13</v>
       </c>
       <c r="Z3" t="n">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4">
@@ -11254,13 +11254,13 @@
         <v>0.823794246666667</v>
       </c>
       <c r="X4" t="n">
-        <v>0.91822495</v>
+        <v>0.9203255</v>
       </c>
       <c r="Y4" t="n">
         <v>11</v>
       </c>
       <c r="Z4" t="n">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5">
@@ -11334,13 +11334,13 @@
         <v>0.78974572</v>
       </c>
       <c r="X5" t="n">
-        <v>0.92385425</v>
+        <v>0.9293631</v>
       </c>
       <c r="Y5" t="n">
         <v>18</v>
       </c>
       <c r="Z5" t="n">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6">
@@ -11414,13 +11414,13 @@
         <v>0.789701633333333</v>
       </c>
       <c r="X6" t="n">
-        <v>0.92385425</v>
+        <v>0.9293631</v>
       </c>
       <c r="Y6" t="n">
         <v>20</v>
       </c>
       <c r="Z6" t="n">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7">
@@ -11494,13 +11494,13 @@
         <v>0.789723493333333</v>
       </c>
       <c r="X7" t="n">
-        <v>0.92385425</v>
+        <v>0.9293631</v>
       </c>
       <c r="Y7" t="n">
         <v>19</v>
       </c>
       <c r="Z7" t="n">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8">
@@ -11574,7 +11574,7 @@
         <v>0.847183286666667</v>
       </c>
       <c r="X8" t="n">
-        <v>0.9280186</v>
+        <v>0.9341104</v>
       </c>
       <c r="Y8" t="n">
         <v>9</v>
@@ -11654,13 +11654,13 @@
         <v>0.8207482</v>
       </c>
       <c r="X9" t="n">
-        <v>0.91829245</v>
+        <v>0.9194454</v>
       </c>
       <c r="Y9" t="n">
         <v>14</v>
       </c>
       <c r="Z9" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10">
@@ -11734,13 +11734,13 @@
         <v>0.8237107</v>
       </c>
       <c r="X10" t="n">
-        <v>0.91822495</v>
+        <v>0.9203255</v>
       </c>
       <c r="Y10" t="n">
         <v>12</v>
       </c>
       <c r="Z10" t="n">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11">
@@ -11814,7 +11814,7 @@
         <v>0.847183286666667</v>
       </c>
       <c r="X11" t="n">
-        <v>0.9280186</v>
+        <v>0.9341104</v>
       </c>
       <c r="Y11" t="n">
         <v>10</v>
@@ -11894,13 +11894,13 @@
         <v>0.8207482</v>
       </c>
       <c r="X12" t="n">
-        <v>0.91829245</v>
+        <v>0.9194454</v>
       </c>
       <c r="Y12" t="n">
         <v>15</v>
       </c>
       <c r="Z12" t="n">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13">
@@ -11974,7 +11974,7 @@
         <v>0.848088613333333</v>
       </c>
       <c r="X13" t="n">
-        <v>0.9263877</v>
+        <v>0.931004</v>
       </c>
       <c r="Y13" t="n">
         <v>1</v>
@@ -12054,7 +12054,7 @@
         <v>0.84759658</v>
       </c>
       <c r="X14" t="n">
-        <v>0.9280186</v>
+        <v>0.9341104</v>
       </c>
       <c r="Y14" t="n">
         <v>4</v>
@@ -12134,13 +12134,13 @@
         <v>0.791082693333333</v>
       </c>
       <c r="X15" t="n">
-        <v>0.9244114</v>
+        <v>0.9293527</v>
       </c>
       <c r="Y15" t="n">
         <v>16</v>
       </c>
       <c r="Z15" t="n">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16">
@@ -12214,7 +12214,7 @@
         <v>0.84758284</v>
       </c>
       <c r="X16" t="n">
-        <v>0.9280186</v>
+        <v>0.9341104</v>
       </c>
       <c r="Y16" t="n">
         <v>5</v>
@@ -12294,7 +12294,7 @@
         <v>0.847823566666667</v>
       </c>
       <c r="X17" t="n">
-        <v>0.92813275</v>
+        <v>0.9343387</v>
       </c>
       <c r="Y17" t="n">
         <v>2</v>
@@ -12374,7 +12374,7 @@
         <v>0.8475148</v>
       </c>
       <c r="X18" t="n">
-        <v>0.9280186</v>
+        <v>0.9341104</v>
       </c>
       <c r="Y18" t="n">
         <v>6</v>
@@ -12454,13 +12454,13 @@
         <v>0.79106726</v>
       </c>
       <c r="X19" t="n">
-        <v>0.9244114</v>
+        <v>0.9293527</v>
       </c>
       <c r="Y19" t="n">
         <v>17</v>
       </c>
       <c r="Z19" t="n">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="20">
@@ -12534,7 +12534,7 @@
         <v>0.847501053333333</v>
       </c>
       <c r="X20" t="n">
-        <v>0.9280186</v>
+        <v>0.9341104</v>
       </c>
       <c r="Y20" t="n">
         <v>7</v>
@@ -12614,7 +12614,7 @@
         <v>0.84768658</v>
       </c>
       <c r="X21" t="n">
-        <v>0.92819105</v>
+        <v>0.9344553</v>
       </c>
       <c r="Y21" t="n">
         <v>3</v>

</xml_diff>